<commit_message>
Added TextRenderer class along with all the resources needed to complile and draw with it.
Amended project output along with includes and libs to support FreeFont.
</commit_message>
<xml_diff>
--- a/Agile.xlsx
+++ b/Agile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Image-Processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C300A89-73A7-498E-8B32-F9CA16C7E833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DAA2971-5F50-45EE-B331-9E1C055E94C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0E935330-A39C-44BE-9F97-B57720268434}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="66">
   <si>
     <t>Sprint</t>
   </si>
@@ -600,7 +600,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,6 +763,9 @@
       </c>
       <c r="C12" s="1" t="s">
         <v>60</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated Application class to singleton. Not integrated yet.
Added FPS text and shader to render text. Currently draws placeholder fps in original video window. This is done in the Helper.h file.

Updated sprint sheet.
</commit_message>
<xml_diff>
--- a/Agile.xlsx
+++ b/Agile.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Image-Processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DAA2971-5F50-45EE-B331-9E1C055E94C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF576C77-A72E-4538-AABA-6EC50B5EBBE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0E935330-A39C-44BE-9F97-B57720268434}"/>
   </bookViews>
   <sheets>
     <sheet name="02_03_24" sheetId="1" r:id="rId1"/>
     <sheet name="02_17_24" sheetId="2" r:id="rId2"/>
-    <sheet name="Tasks" sheetId="3" r:id="rId3"/>
+    <sheet name="Remaining Tasks" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="73">
   <si>
     <t>Sprint</t>
   </si>
@@ -203,9 +203,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Must rework shader and handle image processing class</t>
-  </si>
-  <si>
     <t>Ends</t>
   </si>
   <si>
@@ -225,6 +222,30 @@
   </si>
   <si>
     <t>FPS Counter Shader</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Placeholder </t>
+  </si>
+  <si>
+    <t>Started</t>
+  </si>
+  <si>
+    <t>Must rework shader and handle image processing class.</t>
+  </si>
+  <si>
+    <t>Logger</t>
+  </si>
+  <si>
+    <t>Logger Class</t>
+  </si>
+  <si>
+    <t>Updated all error messages to logger</t>
+  </si>
+  <si>
+    <t>Needs to be singleton.</t>
+  </si>
+  <si>
+    <t>Need to be a singleton.</t>
   </si>
 </sst>
 </file>
@@ -600,7 +621,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,6 +663,9 @@
       <c r="D2" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="E2" s="1" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -667,6 +691,9 @@
       <c r="C4" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -707,7 +734,7 @@
         <v>29</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -762,10 +789,13 @@
         <v>2</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>21</v>
+        <v>66</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -776,7 +806,10 @@
         <v>1</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -787,12 +820,15 @@
         <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>57</v>
@@ -851,10 +887,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66C9FBAC-C701-4031-A327-AA3C3F5B218D}">
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,7 +904,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -948,12 +984,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
@@ -961,32 +997,32 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C23" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C24" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C26" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>19</v>
       </c>
@@ -999,8 +1035,11 @@
       <c r="D28" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" s="1">
         <v>1</v>
       </c>
@@ -1011,7 +1050,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" s="1">
         <v>1</v>
       </c>
@@ -1019,7 +1058,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" s="1">
         <v>2</v>
       </c>
@@ -1030,7 +1069,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" s="1">
         <v>2</v>
       </c>
@@ -1083,7 +1122,7 @@
         <v>1</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1091,7 +1130,7 @@
         <v>1</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1156,7 +1195,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B49" s="1">
         <v>1</v>
       </c>
@@ -1164,7 +1203,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B50" s="1">
         <v>1</v>
       </c>
@@ -1172,7 +1211,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B51" s="1">
         <v>2</v>
       </c>
@@ -1180,7 +1219,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B52" s="1">
         <v>4</v>
       </c>
@@ -1188,39 +1227,58 @@
         <v>47</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C53" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C54" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C55" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C56" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C57" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C58" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C59" s="1" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B62" s="1">
+        <v>1</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B63" s="1">
+        <v>2</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated program to use singleton correctly and switched over fps counter to singleton.
</commit_message>
<xml_diff>
--- a/Agile.xlsx
+++ b/Agile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Image-Processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF576C77-A72E-4538-AABA-6EC50B5EBBE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{245837E2-976F-4577-8125-17F4D960C417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0E935330-A39C-44BE-9F97-B57720268434}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0E935330-A39C-44BE-9F97-B57720268434}"/>
   </bookViews>
   <sheets>
     <sheet name="02_03_24" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="76">
   <si>
     <t>Sprint</t>
   </si>
@@ -215,9 +215,6 @@
     <t>FPS Counter Class</t>
   </si>
   <si>
-    <t>Note: Each point is ~2 hours of work.</t>
-  </si>
-  <si>
     <t>Text Shader</t>
   </si>
   <si>
@@ -246,6 +243,18 @@
   </si>
   <si>
     <t>Need to be a singleton.</t>
+  </si>
+  <si>
+    <t>Displays currently, but does not update in real-time.</t>
+  </si>
+  <si>
+    <t>One Solution.</t>
+  </si>
+  <si>
+    <t>Note: Each point is ~2 hours of work. Status can be 'Started,' 'Implemented,' 'Cleanup' and 'Finished.'</t>
+  </si>
+  <si>
+    <t>Median Filter (3 Color)</t>
   </si>
 </sst>
 </file>
@@ -618,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BE06BE6-C00F-46F9-A856-B354F4C8DB08}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,7 +673,7 @@
         <v>21</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -692,7 +701,7 @@
         <v>23</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -734,7 +743,7 @@
         <v>29</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -769,6 +778,12 @@
       <c r="C10" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="D10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
@@ -792,10 +807,10 @@
         <v>59</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -812,7 +827,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>45325</v>
       </c>
@@ -823,22 +838,36 @@
         <v>61</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="2">
+        <v>45325</v>
+      </c>
+      <c r="B15" s="1">
+        <v>3</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
         <v>45338</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B19" s="1">
         <f>SUM(B2:B12)</f>
         <v>13</v>
       </c>
@@ -890,7 +919,7 @@
   <dimension ref="A1:E63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,7 +933,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -1036,7 +1065,7 @@
         <v>21</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1122,7 +1151,7 @@
         <v>1</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1130,7 +1159,7 @@
         <v>1</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1264,13 +1293,13 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B62" s="1">
+        <v>1</v>
+      </c>
+      <c r="C62" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="B62" s="1">
-        <v>1</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1278,7 +1307,7 @@
         <v>2</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New timer implemented that has slightly less CPU overhead.
Some slight cleanup in the Timer class, Main.cpp, and Application.cpp.
</commit_message>
<xml_diff>
--- a/Agile.xlsx
+++ b/Agile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Image-Processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{245837E2-976F-4577-8125-17F4D960C417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1331D41-4355-45A1-A3DE-4051C9508685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0E935330-A39C-44BE-9F97-B57720268434}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="76">
   <si>
     <t>Sprint</t>
   </si>
@@ -630,7 +630,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,6 +766,9 @@
       </c>
       <c r="C9" s="1" t="s">
         <v>38</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Speed improvement to Gaussian Blur.
</commit_message>
<xml_diff>
--- a/Agile.xlsx
+++ b/Agile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Image-Processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1331D41-4355-45A1-A3DE-4051C9508685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908094B9-3926-47E1-AD1B-8D6B0AB4D03C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0E935330-A39C-44BE-9F97-B57720268434}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{0E935330-A39C-44BE-9F97-B57720268434}"/>
   </bookViews>
   <sheets>
     <sheet name="02_03_24" sheetId="1" r:id="rId1"/>
@@ -630,7 +630,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Clean up of gaussian blur.
Initial implementation of color median filter. Updated controls and GUI to include it.

Change default settings to have better image with current video.
</commit_message>
<xml_diff>
--- a/Agile.xlsx
+++ b/Agile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Image-Processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908094B9-3926-47E1-AD1B-8D6B0AB4D03C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D973CFC1-6B2E-4C9B-B10D-FB2F4252DDEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{0E935330-A39C-44BE-9F97-B57720268434}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="75">
   <si>
     <t>Sprint</t>
   </si>
@@ -221,9 +221,6 @@
     <t>FPS Counter Shader</t>
   </si>
   <si>
-    <t xml:space="preserve">Placeholder </t>
-  </si>
-  <si>
     <t>Started</t>
   </si>
   <si>
@@ -242,12 +239,6 @@
     <t>Needs to be singleton.</t>
   </si>
   <si>
-    <t>Need to be a singleton.</t>
-  </si>
-  <si>
-    <t>Displays currently, but does not update in real-time.</t>
-  </si>
-  <si>
     <t>One Solution.</t>
   </si>
   <si>
@@ -255,6 +246,12 @@
   </si>
   <si>
     <t>Median Filter (3 Color)</t>
+  </si>
+  <si>
+    <t>Need  to be a singleton and have all the pointer's nomenclature updated.</t>
+  </si>
+  <si>
+    <t>Placeholder. Needs to integrate with Resource Manager and be used in Render().</t>
   </si>
 </sst>
 </file>
@@ -630,7 +627,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,7 +656,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>45325</v>
       </c>
@@ -673,7 +670,7 @@
         <v>21</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -701,7 +698,7 @@
         <v>23</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -743,7 +740,7 @@
         <v>29</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -785,7 +782,7 @@
         <v>21</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -799,7 +796,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>45325</v>
       </c>
@@ -810,10 +807,10 @@
         <v>59</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -830,7 +827,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>45325</v>
       </c>
@@ -841,10 +838,7 @@
         <v>61</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>72</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -855,7 +849,10 @@
         <v>3</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -936,7 +933,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -1068,7 +1065,7 @@
         <v>21</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1296,13 +1293,13 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B62" s="1">
+        <v>1</v>
+      </c>
+      <c r="C62" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="B62" s="1">
-        <v>1</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1310,7 +1307,7 @@
         <v>2</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated information in Readme.md.
</commit_message>
<xml_diff>
--- a/Agile.xlsx
+++ b/Agile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Image-Processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D973CFC1-6B2E-4C9B-B10D-FB2F4252DDEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF6A657B-2994-4937-B496-35AF5129C0C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{0E935330-A39C-44BE-9F97-B57720268434}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="76">
   <si>
     <t>Sprint</t>
   </si>
@@ -252,6 +252,9 @@
   </si>
   <si>
     <t>Placeholder. Needs to integrate with Resource Manager and be used in Render().</t>
+  </si>
+  <si>
+    <t>Placeholder general information.</t>
   </si>
 </sst>
 </file>
@@ -627,7 +630,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,6 +797,12 @@
       </c>
       <c r="C11" s="1" t="s">
         <v>55</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Reworked ColorMedian to test against highest/lowest color and luminance.
</commit_message>
<xml_diff>
--- a/Agile.xlsx
+++ b/Agile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Image-Processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF6A657B-2994-4937-B496-35AF5129C0C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99DBF834-406F-4BD2-B8FC-65B1DFC29E9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{0E935330-A39C-44BE-9F97-B57720268434}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="75">
   <si>
     <t>Sprint</t>
   </si>
@@ -140,9 +140,6 @@
     <t>Image Process Class</t>
   </si>
   <si>
-    <t>New Format that needs to be integrated into the resource manager.</t>
-  </si>
-  <si>
     <t>Timer Class</t>
   </si>
   <si>
@@ -215,12 +212,6 @@
     <t>FPS Counter Class</t>
   </si>
   <si>
-    <t>Text Shader</t>
-  </si>
-  <si>
-    <t>FPS Counter Shader</t>
-  </si>
-  <si>
     <t>Started</t>
   </si>
   <si>
@@ -236,9 +227,6 @@
     <t>Updated all error messages to logger</t>
   </si>
   <si>
-    <t>Needs to be singleton.</t>
-  </si>
-  <si>
     <t>One Solution.</t>
   </si>
   <si>
@@ -255,6 +243,15 @@
   </si>
   <si>
     <t>Placeholder general information.</t>
+  </si>
+  <si>
+    <t>Display picture and stop when Video ends</t>
+  </si>
+  <si>
+    <t>Placeholder caution image currently.</t>
+  </si>
+  <si>
+    <t>Integrate into the resource manager.</t>
   </si>
 </sst>
 </file>
@@ -630,7 +627,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,7 +670,7 @@
         <v>21</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -701,7 +698,7 @@
         <v>23</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -743,7 +740,7 @@
         <v>29</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -765,7 +762,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>21</v>
@@ -779,13 +776,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -796,13 +793,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -813,13 +810,13 @@
         <v>2</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -830,7 +827,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>21</v>
@@ -844,7 +841,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>21</v>
@@ -852,24 +849,41 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>45325</v>
+        <v>45329</v>
       </c>
       <c r="B15" s="1">
         <v>3</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>21</v>
       </c>
     </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>45332</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -891,7 +905,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,8 +941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66C9FBAC-C701-4031-A327-AA3C3F5B218D}">
   <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -942,7 +956,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -1022,12 +1036,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
@@ -1035,140 +1049,34 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C23" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C24" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C24" s="1" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C25" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C25" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C26" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B28" s="1">
-        <v>1</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="1">
-        <v>1</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="1">
-        <v>1</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="1">
-        <v>2</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="1">
-        <v>2</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="1">
-        <v>2</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="1">
-        <v>1</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="1">
-        <v>1</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C36" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="1">
-        <v>3</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="1">
-        <v>1</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="1">
-        <v>1</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1222,7 +1130,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B48" s="1">
         <v>2</v>
       </c>
@@ -1230,7 +1138,7 @@
         <v>36</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>37</v>
+        <v>74</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1238,7 +1146,7 @@
         <v>1</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1246,7 +1154,7 @@
         <v>1</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1254,7 +1162,7 @@
         <v>2</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1262,53 +1170,53 @@
         <v>4</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C53" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C54" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C55" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C56" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C57" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C58" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C59" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B62" s="1">
         <v>1</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1316,7 +1224,7 @@
         <v>2</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>